<commit_message>
used csv python to get values from crime data
</commit_message>
<xml_diff>
--- a/data/MASTER_FILE_AKSHAY.xlsx
+++ b/data/MASTER_FILE_AKSHAY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Name of State</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>CRIME TOTAL 2012</t>
+  </si>
+  <si>
+    <t>DOMESTIC 2013</t>
+  </si>
+  <si>
+    <t>FOREIGN 2013</t>
+  </si>
+  <si>
+    <t>HOTEL ROOMS 2013</t>
+  </si>
+  <si>
+    <t>CRIME TOTAL 2013</t>
   </si>
 </sst>
 </file>
@@ -548,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,78 +580,96 @@
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="16" width="14" customWidth="1"/>
+    <col min="14" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" customWidth="1"/>
-    <col min="18" max="20" width="14.5703125" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" customWidth="1"/>
+    <col min="18" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -649,32 +679,56 @@
       <c r="C2">
         <v>12512</v>
       </c>
+      <c r="E2">
+        <v>47</v>
+      </c>
       <c r="F2">
         <v>142042</v>
       </c>
       <c r="G2">
         <v>13684</v>
       </c>
+      <c r="I2">
+        <v>42</v>
+      </c>
       <c r="J2">
         <v>180781</v>
       </c>
       <c r="K2">
         <v>14615</v>
       </c>
+      <c r="M2">
+        <v>57</v>
+      </c>
       <c r="N2">
         <v>202221</v>
       </c>
       <c r="O2">
         <v>15814</v>
       </c>
+      <c r="Q2">
+        <v>58</v>
+      </c>
       <c r="R2">
         <v>238699</v>
       </c>
       <c r="S2">
         <v>17538</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>55</v>
+      </c>
+      <c r="V2">
+        <v>243703</v>
+      </c>
+      <c r="W2">
+        <v>14742</v>
+      </c>
+      <c r="Y2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -684,32 +738,56 @@
       <c r="C3">
         <v>789180</v>
       </c>
+      <c r="E3">
+        <v>4856</v>
+      </c>
       <c r="F3">
         <v>157489927</v>
       </c>
       <c r="G3">
         <v>795173</v>
       </c>
+      <c r="I3">
+        <v>4223</v>
+      </c>
       <c r="J3">
         <v>155789584</v>
       </c>
       <c r="K3">
         <v>322825</v>
       </c>
+      <c r="M3">
+        <v>4523</v>
+      </c>
       <c r="N3">
         <v>153119816</v>
       </c>
       <c r="O3">
         <v>264563</v>
       </c>
+      <c r="Q3">
+        <v>4437</v>
+      </c>
       <c r="R3">
         <v>206817895</v>
       </c>
       <c r="S3">
         <v>292845</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>4408</v>
+      </c>
+      <c r="V3">
+        <v>152102150</v>
+      </c>
+      <c r="W3">
+        <v>223518</v>
+      </c>
+      <c r="Y3">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -725,26 +803,47 @@
       <c r="G4">
         <v>3945</v>
       </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
       <c r="J4">
         <v>227857</v>
       </c>
       <c r="K4">
         <v>3395</v>
       </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
       <c r="N4">
         <v>233227</v>
       </c>
       <c r="O4">
         <v>4753</v>
       </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
       <c r="R4">
         <v>317243</v>
       </c>
       <c r="S4">
         <v>5135</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>125461</v>
+      </c>
+      <c r="W4">
+        <v>10846</v>
+      </c>
+      <c r="Y4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -754,32 +853,56 @@
       <c r="C5">
         <v>14426</v>
       </c>
+      <c r="E5">
+        <v>3393</v>
+      </c>
       <c r="F5">
         <v>3850521</v>
       </c>
       <c r="G5">
         <v>14942</v>
       </c>
+      <c r="I5">
+        <v>3171</v>
+      </c>
       <c r="J5">
         <v>4050924</v>
       </c>
       <c r="K5">
         <v>15157</v>
       </c>
+      <c r="M5">
+        <v>3131</v>
+      </c>
       <c r="N5">
         <v>4339485</v>
       </c>
       <c r="O5">
         <v>16400</v>
       </c>
+      <c r="Q5">
+        <v>2983</v>
+      </c>
       <c r="R5">
         <v>4511407</v>
       </c>
       <c r="S5">
         <v>17543</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>2987</v>
+      </c>
+      <c r="V5">
+        <v>4684527</v>
+      </c>
+      <c r="W5">
+        <v>17638</v>
+      </c>
+      <c r="Y5">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -789,32 +912,56 @@
       <c r="C6">
         <v>345572</v>
       </c>
+      <c r="E6">
+        <v>5279</v>
+      </c>
       <c r="F6">
         <v>15685581</v>
       </c>
       <c r="G6">
         <v>423042</v>
       </c>
+      <c r="I6">
+        <v>4902</v>
+      </c>
       <c r="J6">
         <v>18491804</v>
       </c>
       <c r="K6">
         <v>635722</v>
       </c>
+      <c r="M6">
+        <v>4678</v>
+      </c>
       <c r="N6">
         <v>18397490</v>
       </c>
       <c r="O6">
         <v>972487</v>
       </c>
+      <c r="Q6">
+        <v>4122</v>
+      </c>
       <c r="R6">
         <v>21447099</v>
       </c>
       <c r="S6">
         <v>1096933</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>3622</v>
+      </c>
+      <c r="V6">
+        <v>21588306</v>
+      </c>
+      <c r="W6">
+        <v>765835</v>
+      </c>
+      <c r="Y6">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -824,32 +971,56 @@
       <c r="C7">
         <v>34762</v>
       </c>
+      <c r="E7">
+        <v>136</v>
+      </c>
       <c r="F7">
         <v>914742</v>
       </c>
       <c r="G7">
         <v>37967</v>
       </c>
+      <c r="I7">
+        <v>189</v>
+      </c>
       <c r="J7">
         <v>905450</v>
       </c>
       <c r="K7">
         <v>39333</v>
       </c>
+      <c r="M7">
+        <v>198</v>
+      </c>
       <c r="N7">
         <v>909904</v>
       </c>
       <c r="O7">
         <v>37181</v>
       </c>
+      <c r="Q7">
+        <v>203</v>
+      </c>
       <c r="R7">
         <v>924589</v>
       </c>
       <c r="S7">
         <v>34130</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>209</v>
+      </c>
+      <c r="V7">
+        <v>936922</v>
+      </c>
+      <c r="W7">
+        <v>40124</v>
+      </c>
+      <c r="Y7">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -859,32 +1030,56 @@
       <c r="C8">
         <v>1314</v>
       </c>
+      <c r="E8">
+        <v>4442</v>
+      </c>
       <c r="F8">
         <v>511561</v>
       </c>
       <c r="G8">
         <v>1277</v>
       </c>
+      <c r="I8">
+        <v>4540</v>
+      </c>
       <c r="J8">
         <v>566298</v>
       </c>
       <c r="K8">
         <v>1586</v>
       </c>
+      <c r="M8">
+        <v>4906</v>
+      </c>
       <c r="N8">
         <v>644425</v>
       </c>
       <c r="O8">
         <v>1726</v>
       </c>
+      <c r="Q8">
+        <v>5339</v>
+      </c>
       <c r="R8">
         <v>15036530</v>
       </c>
       <c r="S8">
         <v>4172</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>5511</v>
+      </c>
+      <c r="V8">
+        <v>22801031</v>
+      </c>
+      <c r="W8">
+        <v>3886</v>
+      </c>
+      <c r="Y8">
+        <v>6112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -894,32 +1089,56 @@
       <c r="C9">
         <v>5719</v>
       </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
       <c r="F9">
         <v>506625</v>
       </c>
       <c r="G9">
         <v>7109</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
       <c r="J9">
         <v>495575</v>
       </c>
       <c r="K9">
         <v>1698</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
       <c r="N9">
         <v>422265</v>
       </c>
       <c r="O9">
         <v>1412</v>
       </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
       <c r="R9">
         <v>469213</v>
       </c>
       <c r="S9">
         <v>1234</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>481618</v>
+      </c>
+      <c r="W9">
+        <v>1582</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -929,32 +1148,56 @@
       <c r="C10">
         <v>5266</v>
       </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
       <c r="F10">
         <v>563461</v>
       </c>
       <c r="G10">
         <v>5748</v>
       </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
       <c r="J10">
         <v>774166</v>
       </c>
       <c r="K10">
         <v>5139</v>
       </c>
+      <c r="M10">
+        <v>14</v>
+      </c>
       <c r="N10">
         <v>832906</v>
       </c>
       <c r="O10">
         <v>4484</v>
       </c>
+      <c r="Q10">
+        <v>12</v>
+      </c>
       <c r="R10">
         <v>803963</v>
       </c>
       <c r="S10">
         <v>4607</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>14</v>
+      </c>
+      <c r="V10">
+        <v>819947</v>
+      </c>
+      <c r="W10">
+        <v>4814</v>
+      </c>
+      <c r="Y10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -964,32 +1207,56 @@
       <c r="C11">
         <v>2339287</v>
       </c>
+      <c r="E11">
+        <v>1685</v>
+      </c>
       <c r="F11">
         <v>2041173</v>
       </c>
       <c r="G11">
         <v>1958272</v>
       </c>
+      <c r="I11">
+        <v>1904</v>
+      </c>
       <c r="J11">
         <v>13558353</v>
       </c>
       <c r="K11">
         <v>1893650</v>
       </c>
+      <c r="M11">
+        <v>2350</v>
+      </c>
       <c r="N11">
         <v>15428865</v>
       </c>
       <c r="O11">
         <v>2159925</v>
       </c>
+      <c r="Q11">
+        <v>2703</v>
+      </c>
       <c r="R11">
         <v>18495139</v>
       </c>
       <c r="S11">
         <v>2345980</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>2722</v>
+      </c>
+      <c r="V11">
+        <v>20215187</v>
+      </c>
+      <c r="W11">
+        <v>2301395</v>
+      </c>
+      <c r="Y11">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -999,32 +1266,56 @@
       <c r="C12">
         <v>351123</v>
       </c>
+      <c r="E12">
+        <v>119</v>
+      </c>
       <c r="F12">
         <v>2127063</v>
       </c>
       <c r="G12">
         <v>376640</v>
       </c>
+      <c r="I12">
+        <v>128</v>
+      </c>
       <c r="J12">
         <v>2201752</v>
       </c>
       <c r="K12">
         <v>441053</v>
       </c>
+      <c r="M12">
+        <v>134</v>
+      </c>
       <c r="N12">
         <v>2225002</v>
       </c>
       <c r="O12">
         <v>445935</v>
       </c>
+      <c r="Q12">
+        <v>123</v>
+      </c>
       <c r="R12">
         <v>2337499</v>
       </c>
       <c r="S12">
         <v>450530</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>117</v>
+      </c>
+      <c r="V12">
+        <v>2629151</v>
+      </c>
+      <c r="W12">
+        <v>492322</v>
+      </c>
+      <c r="Y12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1034,32 +1325,56 @@
       <c r="C13">
         <v>110702</v>
       </c>
+      <c r="E13">
+        <v>4337</v>
+      </c>
       <c r="F13">
         <v>15909931</v>
       </c>
       <c r="G13">
         <v>102747</v>
       </c>
+      <c r="I13">
+        <v>3511</v>
+      </c>
       <c r="J13">
         <v>18861296</v>
       </c>
       <c r="K13">
         <v>130739</v>
       </c>
+      <c r="M13">
+        <v>3535</v>
+      </c>
       <c r="N13">
         <v>21017478</v>
       </c>
       <c r="O13">
         <v>166042</v>
       </c>
+      <c r="Q13">
+        <v>3745</v>
+      </c>
       <c r="R13">
         <v>24379023</v>
       </c>
       <c r="S13">
         <v>174150</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>3729</v>
+      </c>
+      <c r="V13">
+        <v>27412517</v>
+      </c>
+      <c r="W13">
+        <v>198773</v>
+      </c>
+      <c r="Y13">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1069,32 +1384,56 @@
       <c r="C14">
         <v>87172</v>
       </c>
+      <c r="E14">
+        <v>4589</v>
+      </c>
       <c r="F14">
         <v>6408423</v>
       </c>
       <c r="G14">
         <v>137094</v>
       </c>
+      <c r="I14">
+        <v>5010</v>
+      </c>
       <c r="J14">
         <v>6915269</v>
       </c>
       <c r="K14">
         <v>106433</v>
       </c>
+      <c r="M14">
+        <v>5471</v>
+      </c>
       <c r="N14">
         <v>5988062</v>
       </c>
       <c r="O14">
         <v>130435</v>
       </c>
+      <c r="Q14">
+        <v>5802</v>
+      </c>
       <c r="R14">
         <v>6799242</v>
       </c>
       <c r="S14">
         <v>233002</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>6024</v>
+      </c>
+      <c r="V14">
+        <v>7128027</v>
+      </c>
+      <c r="W14">
+        <v>228200</v>
+      </c>
+      <c r="Y14">
+        <v>6313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1104,6 +1443,9 @@
       <c r="C15">
         <v>376736</v>
       </c>
+      <c r="E15">
+        <v>663</v>
+      </c>
       <c r="F15">
         <v>11036572</v>
       </c>
@@ -1111,26 +1453,47 @@
         <v>400583</v>
       </c>
       <c r="H15" s="1"/>
+      <c r="I15">
+        <v>638</v>
+      </c>
       <c r="J15">
         <v>12811986</v>
       </c>
       <c r="K15">
         <v>453616</v>
       </c>
+      <c r="M15">
+        <v>717</v>
+      </c>
       <c r="N15">
         <v>14604888</v>
       </c>
       <c r="O15">
         <v>484518</v>
       </c>
+      <c r="Q15">
+        <v>679</v>
+      </c>
       <c r="R15">
         <v>15646048</v>
       </c>
       <c r="S15">
         <v>500284</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>680</v>
+      </c>
+      <c r="V15">
+        <v>14715586</v>
+      </c>
+      <c r="W15">
+        <v>414249</v>
+      </c>
+      <c r="Y15">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1140,32 +1503,56 @@
       <c r="C16">
         <v>54697</v>
       </c>
+      <c r="E16">
+        <v>220</v>
+      </c>
       <c r="F16">
         <v>9234862</v>
       </c>
       <c r="G16">
         <v>54475</v>
       </c>
+      <c r="I16">
+        <v>232</v>
+      </c>
       <c r="J16">
         <v>9973189</v>
       </c>
       <c r="K16">
         <v>48099</v>
       </c>
+      <c r="M16">
+        <v>238</v>
+      </c>
       <c r="N16">
         <v>13071531</v>
       </c>
       <c r="O16">
         <v>71593</v>
       </c>
+      <c r="Q16">
+        <v>235</v>
+      </c>
       <c r="R16">
         <v>12427122</v>
       </c>
       <c r="S16">
         <v>78802</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>294</v>
+      </c>
+      <c r="V16">
+        <v>13642402</v>
+      </c>
+      <c r="W16">
+        <v>60845</v>
+      </c>
+      <c r="Y16">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1175,32 +1562,56 @@
       <c r="C17">
         <v>5803</v>
       </c>
+      <c r="E17">
+        <v>5480</v>
+      </c>
       <c r="F17">
         <v>7610160</v>
       </c>
       <c r="G17">
         <v>8303</v>
       </c>
+      <c r="I17">
+        <v>5339</v>
+      </c>
       <c r="J17">
         <v>6885273</v>
       </c>
       <c r="K17">
         <v>15695</v>
       </c>
+      <c r="M17">
+        <v>4965</v>
+      </c>
       <c r="N17">
         <v>10796286</v>
       </c>
       <c r="O17">
         <v>72467</v>
       </c>
+      <c r="Q17">
+        <v>4103</v>
+      </c>
       <c r="R17">
         <v>20421016</v>
       </c>
       <c r="S17">
         <v>31909</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>3986</v>
+      </c>
+      <c r="V17">
+        <v>20511160</v>
+      </c>
+      <c r="W17">
+        <v>45995</v>
+      </c>
+      <c r="Y17">
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1210,32 +1621,56 @@
       <c r="C18">
         <v>174040</v>
       </c>
+      <c r="E18">
+        <v>3623</v>
+      </c>
       <c r="F18">
         <v>32701647</v>
       </c>
       <c r="G18">
         <v>229733</v>
       </c>
+      <c r="I18">
+        <v>3409</v>
+      </c>
       <c r="J18">
         <v>38202077</v>
       </c>
       <c r="K18">
         <v>380995</v>
       </c>
+      <c r="M18">
+        <v>3598</v>
+      </c>
       <c r="N18">
         <v>84107390</v>
       </c>
       <c r="O18">
         <v>574005</v>
       </c>
+      <c r="Q18">
+        <v>3849</v>
+      </c>
       <c r="R18">
         <v>94052729</v>
       </c>
       <c r="S18">
         <v>595359</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>3960</v>
+      </c>
+      <c r="V18">
+        <v>98010140</v>
+      </c>
+      <c r="W18">
+        <v>636378</v>
+      </c>
+      <c r="Y18">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1245,32 +1680,56 @@
       <c r="C19">
         <v>598929</v>
       </c>
+      <c r="E19">
+        <v>2310</v>
+      </c>
       <c r="F19">
         <v>7789378</v>
       </c>
       <c r="G19">
         <v>548737</v>
       </c>
+      <c r="I19">
+        <v>2450</v>
+      </c>
       <c r="J19">
         <v>8595075</v>
       </c>
       <c r="K19">
         <v>659265</v>
       </c>
+      <c r="M19">
+        <v>2382</v>
+      </c>
       <c r="N19">
         <v>9381455</v>
       </c>
       <c r="O19">
         <v>732985</v>
       </c>
+      <c r="Q19">
+        <v>2041</v>
+      </c>
       <c r="R19">
         <v>10076854</v>
       </c>
       <c r="S19">
         <v>793696</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>2314</v>
+      </c>
+      <c r="V19">
+        <v>10857811</v>
+      </c>
+      <c r="W19">
+        <v>858143</v>
+      </c>
+      <c r="Y19">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1280,32 +1739,56 @@
       <c r="C20">
         <v>1699</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="F20">
         <v>6553</v>
       </c>
       <c r="G20">
         <v>4309</v>
       </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
       <c r="J20">
         <v>7705</v>
       </c>
       <c r="K20">
         <v>1512</v>
       </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="N20">
         <v>9424</v>
       </c>
       <c r="O20">
         <v>567</v>
       </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
       <c r="R20">
         <v>4417</v>
       </c>
       <c r="S20">
         <v>580</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>4784</v>
+      </c>
+      <c r="W20">
+        <v>371</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1315,32 +1798,56 @@
       <c r="C21">
         <v>251733</v>
       </c>
+      <c r="E21">
+        <v>13983</v>
+      </c>
       <c r="F21">
         <v>23106206</v>
       </c>
       <c r="G21">
         <v>200819</v>
       </c>
+      <c r="I21">
+        <v>13395</v>
+      </c>
       <c r="J21">
         <v>38079595</v>
       </c>
       <c r="K21">
         <v>250430</v>
       </c>
+      <c r="M21">
+        <v>12953</v>
+      </c>
       <c r="N21">
         <v>44119820</v>
       </c>
       <c r="O21">
         <v>269559</v>
       </c>
+      <c r="Q21">
+        <v>14434</v>
+      </c>
       <c r="R21">
         <v>53197209</v>
       </c>
       <c r="S21">
         <v>275930</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>14661</v>
+      </c>
+      <c r="V21">
+        <v>63110709</v>
+      </c>
+      <c r="W21">
+        <v>280333</v>
+      </c>
+      <c r="Y21">
+        <v>15494</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1350,32 +1857,56 @@
       <c r="C22">
         <v>2056913</v>
       </c>
+      <c r="E22">
+        <v>7980</v>
+      </c>
       <c r="F22">
         <v>23739130</v>
       </c>
       <c r="G22">
         <v>1999320</v>
       </c>
+      <c r="I22">
+        <v>7556</v>
+      </c>
       <c r="J22">
         <v>48465492</v>
       </c>
       <c r="K22">
         <v>5083126</v>
       </c>
+      <c r="M22">
+        <v>7509</v>
+      </c>
       <c r="N22">
         <v>55333467</v>
       </c>
       <c r="O22">
         <v>4815421</v>
       </c>
+      <c r="Q22">
+        <v>7159</v>
+      </c>
       <c r="R22">
         <v>66330229</v>
       </c>
       <c r="S22">
         <v>5120287</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>7110</v>
+      </c>
+      <c r="V22">
+        <v>82700556</v>
+      </c>
+      <c r="W22">
+        <v>4156343</v>
+      </c>
+      <c r="Y22">
+        <v>7315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1385,32 +1916,56 @@
       <c r="C23">
         <v>354</v>
       </c>
+      <c r="E23">
+        <v>31</v>
+      </c>
       <c r="F23">
         <v>124229</v>
       </c>
       <c r="G23">
         <v>337</v>
       </c>
+      <c r="I23">
+        <v>28</v>
+      </c>
       <c r="J23">
         <v>114062</v>
       </c>
       <c r="K23">
         <v>389</v>
       </c>
+      <c r="M23">
+        <v>29</v>
+      </c>
       <c r="N23">
         <v>134505</v>
       </c>
       <c r="O23">
         <v>578</v>
       </c>
+      <c r="Q23">
+        <v>23</v>
+      </c>
       <c r="R23">
         <v>134541</v>
       </c>
       <c r="S23">
         <v>749</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>23</v>
+      </c>
+      <c r="V23">
+        <v>140673</v>
+      </c>
+      <c r="W23">
+        <v>1908</v>
+      </c>
+      <c r="Y23">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1420,32 +1975,56 @@
       <c r="C24">
         <v>4919</v>
       </c>
+      <c r="E24">
+        <v>60</v>
+      </c>
       <c r="F24">
         <v>591398</v>
       </c>
       <c r="G24">
         <v>4522</v>
       </c>
+      <c r="I24">
+        <v>77</v>
+      </c>
       <c r="J24">
         <v>652756</v>
       </c>
       <c r="K24">
         <v>4177</v>
       </c>
+      <c r="M24">
+        <v>48</v>
+      </c>
       <c r="N24">
         <v>667504</v>
       </c>
       <c r="O24">
         <v>4803</v>
       </c>
+      <c r="Q24">
+        <v>54</v>
+      </c>
       <c r="R24">
         <v>680254</v>
       </c>
       <c r="S24">
         <v>5313</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>62</v>
+      </c>
+      <c r="V24">
+        <v>691269</v>
+      </c>
+      <c r="W24">
+        <v>6773</v>
+      </c>
+      <c r="Y24">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1455,32 +2034,56 @@
       <c r="C25">
         <v>902</v>
       </c>
+      <c r="E25">
+        <v>210</v>
+      </c>
       <c r="F25">
         <v>56651</v>
       </c>
       <c r="G25">
         <v>513</v>
       </c>
+      <c r="I25">
+        <v>235</v>
+      </c>
       <c r="J25">
         <v>57292</v>
       </c>
       <c r="K25">
         <v>731</v>
       </c>
+      <c r="M25">
+        <v>275</v>
+      </c>
       <c r="N25">
         <v>62174</v>
       </c>
       <c r="O25">
         <v>658</v>
       </c>
+      <c r="Q25">
+        <v>265</v>
+      </c>
       <c r="R25">
         <v>64249</v>
       </c>
       <c r="S25">
         <v>744</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>248</v>
+      </c>
+      <c r="V25">
+        <v>63377</v>
+      </c>
+      <c r="W25">
+        <v>800</v>
+      </c>
+      <c r="Y25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1490,32 +2093,56 @@
       <c r="C26">
         <v>1209</v>
       </c>
+      <c r="E26">
+        <v>112</v>
+      </c>
       <c r="F26">
         <v>20953</v>
       </c>
       <c r="G26">
         <v>1423</v>
       </c>
+      <c r="I26">
+        <v>126</v>
+      </c>
       <c r="J26">
         <v>21094</v>
       </c>
       <c r="K26">
         <v>1132</v>
       </c>
+      <c r="M26">
+        <v>110</v>
+      </c>
       <c r="N26">
         <v>25391</v>
       </c>
       <c r="O26">
         <v>2080</v>
       </c>
+      <c r="Q26">
+        <v>110</v>
+      </c>
       <c r="R26">
         <v>35915</v>
       </c>
       <c r="S26">
         <v>2489</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>117</v>
+      </c>
+      <c r="V26">
+        <v>35638</v>
+      </c>
+      <c r="W26">
+        <v>3304</v>
+      </c>
+      <c r="Y26">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1525,32 +2152,56 @@
       <c r="C27">
         <v>43966</v>
       </c>
+      <c r="E27">
+        <v>4169</v>
+      </c>
       <c r="F27">
         <v>6891510</v>
       </c>
       <c r="G27">
         <v>45684</v>
       </c>
+      <c r="I27">
+        <v>3926</v>
+      </c>
       <c r="J27">
         <v>7591615</v>
       </c>
       <c r="K27">
         <v>50432</v>
       </c>
+      <c r="M27">
+        <v>3854</v>
+      </c>
       <c r="N27">
         <v>8271257</v>
       </c>
       <c r="O27">
         <v>60722</v>
       </c>
+      <c r="Q27">
+        <v>3521</v>
+      </c>
       <c r="R27">
         <v>9052871</v>
       </c>
       <c r="S27">
         <v>64719</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>3436</v>
+      </c>
+      <c r="V27">
+        <v>9800135</v>
+      </c>
+      <c r="W27">
+        <v>66675</v>
+      </c>
+      <c r="Y27">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1560,32 +2211,56 @@
       <c r="C28">
         <v>6869</v>
       </c>
+      <c r="E28">
+        <v>96</v>
+      </c>
       <c r="F28">
         <v>457240</v>
       </c>
       <c r="G28">
         <v>3184</v>
       </c>
+      <c r="I28">
+        <v>118</v>
+      </c>
       <c r="J28">
         <v>835872</v>
       </c>
       <c r="K28">
         <v>50964</v>
       </c>
+      <c r="M28">
+        <v>129</v>
+      </c>
       <c r="N28">
         <v>897896</v>
       </c>
       <c r="O28">
         <v>52298</v>
       </c>
+      <c r="Q28">
+        <v>129</v>
+      </c>
       <c r="R28">
         <v>981714</v>
       </c>
       <c r="S28">
         <v>52931</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>109</v>
+      </c>
+      <c r="V28">
+        <v>1000277</v>
+      </c>
+      <c r="W28">
+        <v>42624</v>
+      </c>
+      <c r="Y28">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1595,32 +2270,56 @@
       <c r="C29">
         <v>60309</v>
       </c>
+      <c r="E29">
+        <v>3397</v>
+      </c>
       <c r="F29">
         <v>851192</v>
       </c>
       <c r="G29">
         <v>54039</v>
       </c>
+      <c r="I29">
+        <v>3949</v>
+      </c>
       <c r="J29">
         <v>10583509</v>
       </c>
       <c r="K29">
         <v>137122</v>
       </c>
+      <c r="M29">
+        <v>5067</v>
+      </c>
       <c r="N29">
         <v>16416638</v>
       </c>
       <c r="O29">
         <v>150958</v>
       </c>
+      <c r="Q29">
+        <v>5582</v>
+      </c>
       <c r="R29">
         <v>19056143</v>
       </c>
       <c r="S29">
         <v>143805</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>4905</v>
+      </c>
+      <c r="V29">
+        <v>21340888</v>
+      </c>
+      <c r="W29">
+        <v>204074</v>
+      </c>
+      <c r="Y29">
+        <v>5886</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1630,32 +2329,56 @@
       <c r="C30">
         <v>1477646</v>
       </c>
+      <c r="E30">
+        <v>5471</v>
+      </c>
       <c r="F30">
         <v>25558691</v>
       </c>
       <c r="G30">
         <v>1073414</v>
       </c>
+      <c r="I30">
+        <v>5685</v>
+      </c>
       <c r="J30">
         <v>25543877</v>
       </c>
       <c r="K30">
         <v>1278523</v>
       </c>
+      <c r="M30">
+        <v>5285</v>
+      </c>
       <c r="N30">
         <v>27137323</v>
       </c>
       <c r="O30">
         <v>1351974</v>
       </c>
+      <c r="Q30">
+        <v>5169</v>
+      </c>
       <c r="R30">
         <v>28611831</v>
       </c>
       <c r="S30">
         <v>1451370</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>4956</v>
+      </c>
+      <c r="V30">
+        <v>30298150</v>
+      </c>
+      <c r="W30">
+        <v>1437162</v>
+      </c>
+      <c r="Y30">
+        <v>5319</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1665,32 +2388,56 @@
       <c r="C31">
         <v>19154</v>
       </c>
+      <c r="E31">
+        <v>62</v>
+      </c>
       <c r="F31">
         <v>547810</v>
       </c>
       <c r="G31">
         <v>17730</v>
       </c>
+      <c r="I31">
+        <v>65</v>
+      </c>
       <c r="J31">
         <v>700011</v>
       </c>
       <c r="K31">
         <v>20757</v>
       </c>
+      <c r="M31">
+        <v>67</v>
+      </c>
       <c r="N31">
         <v>552453</v>
       </c>
       <c r="O31">
         <v>23602</v>
       </c>
+      <c r="Q31">
+        <v>63</v>
+      </c>
       <c r="R31">
         <v>558538</v>
       </c>
       <c r="S31">
         <v>26489</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>75</v>
+      </c>
+      <c r="V31">
+        <v>576749</v>
+      </c>
+      <c r="W31">
+        <v>31698</v>
+      </c>
+      <c r="Y31">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1700,32 +2447,56 @@
       <c r="C32">
         <v>2029410</v>
       </c>
+      <c r="E32">
+        <v>4971</v>
+      </c>
       <c r="F32">
         <v>115755800</v>
       </c>
       <c r="G32">
         <v>2369050</v>
       </c>
+      <c r="I32">
+        <v>4771</v>
+      </c>
       <c r="J32">
         <v>119188187</v>
       </c>
       <c r="K32">
         <v>2804504</v>
       </c>
+      <c r="M32">
+        <v>4873</v>
+      </c>
       <c r="N32">
         <v>137512991</v>
       </c>
       <c r="O32">
         <v>3373870</v>
       </c>
+      <c r="Q32">
+        <v>4816</v>
+      </c>
       <c r="R32">
         <v>184136840</v>
       </c>
       <c r="S32">
         <v>3561740</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>4508</v>
+      </c>
+      <c r="V32">
+        <v>244232487</v>
+      </c>
+      <c r="W32">
+        <v>3990490</v>
+      </c>
+      <c r="Y32">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1735,32 +2506,56 @@
       <c r="C33">
         <v>3577</v>
       </c>
+      <c r="E33">
+        <v>806</v>
+      </c>
       <c r="F33">
         <v>317541</v>
       </c>
       <c r="G33">
         <v>4246</v>
       </c>
+      <c r="I33">
+        <v>624</v>
+      </c>
       <c r="J33">
         <v>342273</v>
       </c>
       <c r="K33">
         <v>5212</v>
       </c>
+      <c r="M33">
+        <v>547</v>
+      </c>
       <c r="N33">
         <v>359515</v>
       </c>
       <c r="O33">
         <v>6046</v>
       </c>
+      <c r="Q33">
+        <v>529</v>
+      </c>
       <c r="R33">
         <v>361786</v>
       </c>
       <c r="S33">
         <v>7840</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>530</v>
+      </c>
+      <c r="V33">
+        <v>359586</v>
+      </c>
+      <c r="W33">
+        <v>11853</v>
+      </c>
+      <c r="Y33">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1770,32 +2565,56 @@
       <c r="C34">
         <v>1610089</v>
       </c>
+      <c r="E34">
+        <v>18202</v>
+      </c>
       <c r="F34">
         <v>134831852</v>
       </c>
       <c r="G34">
         <v>1532573</v>
       </c>
+      <c r="I34">
+        <v>21872</v>
+      </c>
       <c r="J34">
         <v>144754977</v>
       </c>
       <c r="K34">
         <v>1732707</v>
       </c>
+      <c r="M34">
+        <v>22948</v>
+      </c>
       <c r="N34">
         <v>155430364</v>
       </c>
       <c r="O34">
         <v>1887095</v>
       </c>
+      <c r="Q34">
+        <v>23910</v>
+      </c>
       <c r="R34">
         <v>168381276</v>
       </c>
       <c r="S34">
         <v>1994495</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>22599</v>
+      </c>
+      <c r="V34">
+        <v>226531091</v>
+      </c>
+      <c r="W34">
+        <v>2054420</v>
+      </c>
+      <c r="Y34">
+        <v>23179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1805,32 +2624,56 @@
       <c r="C35">
         <v>99910</v>
       </c>
+      <c r="E35">
+        <v>1031</v>
+      </c>
       <c r="F35">
         <v>21934567</v>
       </c>
       <c r="G35">
         <v>106470</v>
       </c>
+      <c r="I35">
+        <v>1098</v>
+      </c>
       <c r="J35">
         <v>30206030</v>
       </c>
       <c r="K35">
         <v>127258</v>
       </c>
+      <c r="M35">
+        <v>1183</v>
+      </c>
       <c r="N35">
         <v>25946254</v>
       </c>
       <c r="O35">
         <v>124653</v>
       </c>
+      <c r="Q35">
+        <v>1405</v>
+      </c>
       <c r="R35">
         <v>26827329</v>
       </c>
       <c r="S35">
         <v>124555</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>1387</v>
+      </c>
+      <c r="V35">
+        <v>19941128</v>
+      </c>
+      <c r="W35">
+        <v>97683</v>
+      </c>
+      <c r="Y35">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1840,29 +2683,53 @@
       <c r="C36">
         <v>1133671</v>
       </c>
+      <c r="E36">
+        <v>4540</v>
+      </c>
       <c r="F36">
         <v>20528534</v>
       </c>
       <c r="G36">
         <v>1180418</v>
       </c>
+      <c r="I36">
+        <v>4306</v>
+      </c>
       <c r="J36">
         <v>21072324</v>
       </c>
       <c r="K36">
         <v>1192187</v>
       </c>
+      <c r="M36">
+        <v>4415</v>
+      </c>
       <c r="N36">
         <v>22256968</v>
       </c>
       <c r="O36">
         <v>1213270</v>
       </c>
+      <c r="Q36">
+        <v>4379</v>
+      </c>
       <c r="R36">
         <v>22730205</v>
       </c>
       <c r="S36">
         <v>1219610</v>
+      </c>
+      <c r="U36">
+        <v>4639</v>
+      </c>
+      <c r="V36">
+        <v>25547300</v>
+      </c>
+      <c r="W36">
+        <v>1245230</v>
+      </c>
+      <c r="Y36">
+        <v>4388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>